<commit_message>
chandged the logic in main.py
updated the code to include and section to view crops and gives a description about each crop, another section to add crops with calculated profits
</commit_message>
<xml_diff>
--- a/data/crops.xlsx
+++ b/data/crops.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>Season</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Field Size (acres)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Profit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,15 +476,135 @@
           <t>Wheat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="C2" t="n">
+        <v>100</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Rabi</t>
         </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>neil</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wheat</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>rabi</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>neil</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wheat</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>rabi</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>neil</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>xyz</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>neil</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>wheat</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>rabi</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>neil</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>rice</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>kharif</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>90</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2250000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some main.py bugs in the code
</commit_message>
<xml_diff>
--- a/data/crops.xlsx
+++ b/data/crops.xlsx
@@ -82,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,19 +146,16 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -476,11 +473,11 @@
     <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -516,7 +513,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -532,7 +529,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -571,7 +568,7 @@
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -580,14 +577,14 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">

</xml_diff>